<commit_message>
added the scraper.py file
</commit_message>
<xml_diff>
--- a/output/google_maps_data_dentist_in_New_Delhi.xlsx
+++ b/output/google_maps_data_dentist_in_New_Delhi.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,11 +464,6 @@
           <t>reviews_average</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr"/>
@@ -491,30 +486,28 @@
       <c r="F2" t="n">
         <v>4.7</v>
       </c>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lower Ground Floor, SDA Market, opposite IIT Delhi, Block C 5, Hauz Khas Enclave, Hauz Khas, New Delhi, Delhi 110016</t>
+          <t>D-1065, Block D, Friends Colony East, New Friends Colony, New Delhi, Delhi 110065</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>dochomeindia.in</t>
+          <t>dentalclinicdelhi.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>089104 70711</t>
+          <t>011 4051 8978</t>
         </is>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>4.9</v>
       </c>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -537,7 +530,6 @@
       <c r="F4" t="n">
         <v>4.9</v>
       </c>
-      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -560,7 +552,6 @@
       <c r="F5" t="n">
         <v>4.8</v>
       </c>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -583,352 +574,28 @@
       <c r="F6" t="n">
         <v>4.9</v>
       </c>
-      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
-          <t>B-7, 1st Floor, Rajouri Garden (Black Building Chowk, opp. Metro Pillar No. 381, Raja Garden, New Delhi, Delhi 110027</t>
+          <t>Dr Sahni's Dental Clinic, 66, near Friends Club Limited, Friends Colony West, Block A, New Friends Colony, New Delhi, Delhi 110065</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>drbhutanidentalclinic.com</t>
+          <t>drsahnisdental.com</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>088513 29647</t>
+          <t>011 4162 7127</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Dr Sahni's Dental Clinic, 66, near Friends Club Limited, Friends Colony West, Block A, New Friends Colony, New Delhi, Delhi 110065</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>drsahnisdental.com</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>011 4162 7127</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="n">
         <v>4.9</v>
       </c>
-      <c r="G8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr"/>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Shop no-U22_JCS Concourse level, R K ashram, metro station, Panchkuian Marg, Block 42, DIZ Area, Gole Market, New Delhi, Delhi 110001</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>drashokdentistree.com</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>099990 82836</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>B, DDA MARKET, 10, next to Nirula's Block, Pocket 10, Sector B, Vasant Kunj, New Delhi, Delhi 110070</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>clovedental.in</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>095992 16884</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>R-721, Block R, Rajender Nagar Part 1, New Rajinder Nagar, New Delhi, Delhi, 110060</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>thecaringtouch.in</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>085955 19245</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="G11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>K, 35-B, Firoz Ghandi Marg, Block K, Lajpat Nagar II, Lajpat Nagar, New Delhi, Delhi 110024</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>madandental.com</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>098183 31692</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="G12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>9A/1, East Patel Nagar, Patel Nagar, New Delhi, Delhi, 110008</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>kidsdentistdelhi.com</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>098680 78357</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="G13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>47, Masjid Rd, Bhogal, Jangpura, New Delhi, Delhi 110014</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>drarorasdentistry.in</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>074284 47608</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="n">
-        <v>5</v>
-      </c>
-      <c r="G14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>54, shop, South Patel Nagar, Block 8, Patel Nagar, New Delhi, Delhi 110008</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>kailashdental.com</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>081788 44190</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>P-83 Basement, South Extension II, Block P, New Delhi, Delhi 110049</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>merakidentalstudio.com</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>011 4160 6066</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="G16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr"/>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>E-11, Lala Lajpat Rai Rd, near Kailash Colony Metro Station, opp. Metro Pillar no. 77, Block E, East of Kailash, New Delhi, Delhi, 110065</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>dentifique.in</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>087009 09716</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>5</v>
-      </c>
-      <c r="G17" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr"/>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Teeth &amp; More, A2/25, नौरोजी नगर मार्ग, Block A 2, Safdarjung Enclave, New Delhi, Delhi 110029</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>delhidentistspa.com</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>099904 91199</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G18" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr"/>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>B-4/76, B4 Block, Safdarjung Enclave, New Delhi, Delhi 110029</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>newdelhidentalclinic.com</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>087663 86694</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="G19" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr"/>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>E-14, Ground Floor, Rajeshwar Arya Marg, South Extension I, Block E, New Delhi, Delhi 110049</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>abhirachnadental.com</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>011 4140 3700</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="n">
-        <v>5</v>
-      </c>
-      <c r="G20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr"/>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>B-18, Balbir Saxena Marg, Block B, Gulmohar Park, New Delhi, Delhi 110049</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ad.dentally.in</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>092666 65081</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="n">
-        <v>4.9</v>
-      </c>
-      <c r="G21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>